<commit_message>
Add local data copies for manipulations
Copy all the meaningful data from 3 HT databases
</commit_message>
<xml_diff>
--- a/Implied Volatility/ImplicitVolatilityExample/Volatility Example.xlsx
+++ b/Implied Volatility/ImplicitVolatilityExample/Volatility Example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stf2jh.MCINTIRE\Desktop\My Safe Space\Implied Volatility\ImplicitVolatilityExample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Spring 2016\IT_Finance\Project\Implied Volatility\ImplicitVolatilityExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9855" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23670" windowHeight="8400"/>
   </bookViews>
   <sheets>
     <sheet name="Volatility" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,29 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -935,7 +957,12 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -952,13 +979,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1CDFF6F4B1AA2114E1B1BDFB17E42BC45E7111"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2A9CBB267208EC242CA298D6268AAF7BD0DCC2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="5318"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="5054"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -969,13 +996,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2A9CBB267208EC242CA298D6268AAF7BD0DCC2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1CDFF6F4B1AA2114E1B1BDFB17E42BC45E7111"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="5054"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="5318"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1249,42 +1276,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:I22" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:I22" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="B2:I22"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Date" dataDxfId="30"/>
-    <tableColumn id="2" name="Symbol" dataDxfId="29"/>
-    <tableColumn id="3" name="Bid" dataDxfId="28" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Ask" dataDxfId="27" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Strike" dataDxfId="26" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Expiration" dataDxfId="25"/>
-    <tableColumn id="7" name="Type" dataDxfId="24"/>
-    <tableColumn id="8" name="Underlier" dataDxfId="23"/>
+    <tableColumn id="1" name="Date" dataDxfId="32"/>
+    <tableColumn id="2" name="Symbol" dataDxfId="31"/>
+    <tableColumn id="3" name="Bid" dataDxfId="30" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ask" dataDxfId="29" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Strike" dataDxfId="28" dataCellStyle="Currency"/>
+    <tableColumn id="6" name="Expiration" dataDxfId="27"/>
+    <tableColumn id="7" name="Type" dataDxfId="26"/>
+    <tableColumn id="8" name="Underlier" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B25:G26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B25:G26" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="B25:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="19"/>
-    <tableColumn id="2" name="Ticker" dataDxfId="18"/>
-    <tableColumn id="3" name="Bid" dataDxfId="17" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Ask" dataDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="DivDate" dataDxfId="15" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Dividend" dataDxfId="14"/>
+    <tableColumn id="1" name="Date" dataDxfId="21"/>
+    <tableColumn id="2" name="Ticker" dataDxfId="20"/>
+    <tableColumn id="3" name="Bid" dataDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ask" dataDxfId="18" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="DivDate" dataDxfId="17" dataCellStyle="Currency"/>
+    <tableColumn id="6" name="Dividend" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="K2:K22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="K2:K22" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="K2:K22"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Volatility" dataDxfId="10">
+    <tableColumn id="1" name="Volatility" dataDxfId="12">
       <calculatedColumnFormula>$G$28</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1293,26 +1320,26 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="L2:R22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="L2:R22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="L2:R22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="mtm" dataDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="1" name="mtm" dataDxfId="8" dataCellStyle="Currency">
       <calculatedColumnFormula>(Table2[[#This Row],[Bid]]+Table2[[#This Row],[Ask]])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="t" dataDxfId="5">
+    <tableColumn id="2" name="t" dataDxfId="7">
       <calculatedColumnFormula>(Table2[[#This Row],[Expiration]]-Table2[[#This Row],[Date]])/365.25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="d1" dataDxfId="4">
+    <tableColumn id="3" name="d1" dataDxfId="6">
       <calculatedColumnFormula>(LN($L$26/Table2[[#This Row],[Strike]])+($C$28+Table4[[#This Row],[Volatility]]^2/2)*M3)/(Table4[[#This Row],[Volatility]]*SQRT(M3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="d2" dataDxfId="3">
+    <tableColumn id="4" name="d2" dataDxfId="5">
       <calculatedColumnFormula>N3-Table4[[#This Row],[Volatility]]*SQRT(M3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Call price" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="PutPrice" dataDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="5" name="Call price" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="6" name="PutPrice" dataDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>-$L$26*_xlfn.NORM.S.DIST(-N3,TRUE)+Table2[[#This Row],[Strike]]*EXP(-$C$28*M3)*_xlfn.NORM.S.DIST(-O3, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Difference" dataDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="7" name="Difference" dataDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>ABS(Q3-L3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1610,8 +1637,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2995,8 +3022,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="1026" r:id="rId4" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>18</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId4" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId6" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>10</xdr:col>
@@ -3015,32 +3067,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>771525</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="1025" r:id="rId6" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>